<commit_message>
courseleafPatchNew - 3.5.11 initial
</commit_message>
<xml_diff>
--- a/workbooks/courseleafPatchControlNew.xlsx
+++ b/workbooks/courseleafPatchControlNew.xlsx
@@ -9,16 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23745" windowHeight="10665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="-Instructions" sheetId="6" r:id="rId1"/>
     <sheet name="cat" sheetId="1" r:id="rId2"/>
     <sheet name="cim" sheetId="2" r:id="rId3"/>
     <sheet name="cgis" sheetId="10" r:id="rId4"/>
-    <sheet name="pdfgen" sheetId="9" r:id="rId5"/>
-    <sheet name="formbuilder" sheetId="8" r:id="rId6"/>
-    <sheet name="-Include-CGIs" sheetId="7" state="hidden" r:id="rId7"/>
+    <sheet name="-Include-CGIs" sheetId="7" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="91">
   <si>
     <t>git</t>
   </si>
@@ -317,7 +315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1474,7 +1472,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="37" t="s">
         <v>23</v>
       </c>
@@ -1495,10 +1493,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:D25"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,154 +1557,232 @@
       </c>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="A8" s="16"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="A9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="11"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>17</v>
+      <c r="A11" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="25" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
+      <c r="A15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="11"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1717,10 +1793,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,13 +1835,17 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -1792,50 +1872,56 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="28"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1848,7 +1934,7 @@
   <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,175 +2047,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="25"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="25"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="D9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D4"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D15"/>
   <sheetViews>

</xml_diff>